<commit_message>
Minor reformatting for import
</commit_message>
<xml_diff>
--- a/tabular/Asian_SEA1a_miss.xlsx
+++ b/tabular/Asian_SEA1a_miss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathr\Dropbox\GLUE\Whole clades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/general/NCBI-RABV-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE42E9D-8807-4996-9312-D615EAB5BFD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4553EC9D-4EAB-BF44-BAE6-61E2B79838A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="43960" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="110">
   <si>
     <t>sequence.sequenceID</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -496,11 +502,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -520,31 +537,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9FEDFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -915,34 +913,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI17"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH17" sqref="A1:AH17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="18" max="18" width="14.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
-    <col min="22" max="22" width="21.140625" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" customWidth="1"/>
-    <col min="24" max="24" width="23.7109375" customWidth="1"/>
-    <col min="25" max="25" width="26.42578125" customWidth="1"/>
-    <col min="26" max="26" width="22" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" customWidth="1"/>
-    <col min="30" max="30" width="19.85546875" customWidth="1"/>
-    <col min="31" max="31" width="15.28515625" customWidth="1"/>
-    <col min="32" max="32" width="10" customWidth="1"/>
-    <col min="33" max="33" width="17" customWidth="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="12.5" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="21" max="21" width="21.1640625" customWidth="1"/>
+    <col min="22" max="22" width="23.83203125" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" customWidth="1"/>
+    <col min="24" max="24" width="26.5" customWidth="1"/>
+    <col min="25" max="25" width="22" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" customWidth="1"/>
+    <col min="27" max="27" width="11.5" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" customWidth="1"/>
+    <col min="29" max="29" width="19.83203125" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="17" customWidth="1"/>
+    <col min="33" max="33" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -988,59 +989,62 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="AE1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="AH1" s="19" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1089,57 +1093,57 @@
       <c r="P2" t="s">
         <v>74</v>
       </c>
+      <c r="Q2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="R2" s="5" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="V2" s="6">
+        <v>99</v>
+      </c>
+      <c r="U2" s="6">
         <v>1986</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="6">
+      <c r="W2" s="6">
         <v>1986</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="7">
+      <c r="Y2" s="7">
         <v>1986</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AD2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="AE2" s="5" t="s">
         <v>102</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG2" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1188,57 +1192,57 @@
       <c r="P3" t="s">
         <v>75</v>
       </c>
+      <c r="Q3" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R3" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V3" s="10">
+        <v>99</v>
+      </c>
+      <c r="U3" s="10">
         <v>1986</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="X3" s="10">
+      <c r="W3" s="10">
         <v>1986</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="X3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Y3" s="11">
         <v>1986</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AA3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AB3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AD3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE3" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF3" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG3" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1287,59 +1291,59 @@
       <c r="P4" t="s">
         <v>76</v>
       </c>
+      <c r="Q4" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="R4" s="13" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V4" s="10">
+        <v>99</v>
+      </c>
+      <c r="U4" s="10">
         <v>2005</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="V4" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="X4" s="10">
+      <c r="W4" s="10">
         <v>2005</v>
       </c>
-      <c r="Y4" s="13" t="s">
+      <c r="X4" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="Y4" s="13">
         <v>2005</v>
       </c>
-      <c r="AA4" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB4" s="14" t="s">
+      <c r="Z4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AC4" s="13" t="s">
+      <c r="AB4" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AD4" s="14" t="s">
+      <c r="AC4" s="14" t="s">
         <v>104</v>
       </c>
+      <c r="AD4" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE4" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF4" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG4" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="AH4" s="15" t="s">
+      <c r="AG4" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1388,60 +1392,60 @@
       <c r="P5" t="s">
         <v>77</v>
       </c>
+      <c r="Q5" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R5" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="X5" s="10">
+        <v>99</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="W5" s="10">
         <v>2004</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Z5" s="9">
+      <c r="Y5" s="9">
         <v>2005</v>
       </c>
-      <c r="AA5" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB5" s="10" t="s">
+      <c r="Z5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA5" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AD5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE5" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH5" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG5" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1490,60 +1494,60 @@
       <c r="P6" t="s">
         <v>78</v>
       </c>
+      <c r="Q6" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="R6" s="13" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="U6" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="X6" s="10">
+        <v>99</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="W6" s="10">
         <v>2004</v>
       </c>
-      <c r="Y6" s="13" t="s">
+      <c r="X6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="Y6" s="13">
         <v>2005</v>
       </c>
-      <c r="AA6" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB6" s="10" t="s">
+      <c r="Z6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AC6" s="13" t="s">
+      <c r="AB6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AD6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE6" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF6" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH6" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1592,60 +1596,60 @@
       <c r="P7" t="s">
         <v>79</v>
       </c>
+      <c r="Q7" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R7" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="U7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V7" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="X7" s="10">
+        <v>99</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="W7" s="10">
         <v>2004</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="X7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Z7" s="9">
+      <c r="Y7" s="9">
         <v>2005</v>
       </c>
-      <c r="AA7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB7" s="10" t="s">
+      <c r="Z7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AC7" s="9" t="s">
+      <c r="AB7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AD7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE7" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF7" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH7" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG7" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1694,60 +1698,60 @@
       <c r="P8" t="s">
         <v>80</v>
       </c>
+      <c r="Q8" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="R8" s="13" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="U8" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="W8" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="X8" s="10">
+        <v>99</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="W8" s="10">
         <v>2004</v>
       </c>
-      <c r="Y8" s="13" t="s">
+      <c r="X8" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Y8" s="13">
         <v>2005</v>
       </c>
-      <c r="AA8" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB8" s="10" t="s">
+      <c r="Z8" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AC8" s="13" t="s">
+      <c r="AB8" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AD8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE8" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF8" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG8" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH8" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG8" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1796,60 +1800,60 @@
       <c r="P9" t="s">
         <v>81</v>
       </c>
+      <c r="Q9" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R9" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="U9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="X9" s="10">
+        <v>99</v>
+      </c>
+      <c r="U9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="W9" s="10">
         <v>2004</v>
       </c>
-      <c r="Y9" s="9" t="s">
+      <c r="X9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="Y9" s="9">
         <v>2005</v>
       </c>
-      <c r="AA9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB9" s="10" t="s">
+      <c r="Z9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA9" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AC9" s="9" t="s">
+      <c r="AB9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AD9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE9" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF9" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG9" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH9" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG9" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1898,57 +1902,57 @@
       <c r="P10" t="s">
         <v>75</v>
       </c>
+      <c r="Q10" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="R10" s="13" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="U10" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V10" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="W10" s="13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="X10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y10" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z10" s="13">
+        <v>99</v>
+      </c>
+      <c r="Y10" s="13">
         <v>2007</v>
       </c>
+      <c r="Z10" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="AA10" s="13" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="AB10" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC10" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD10" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE10" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF10" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG10" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1997,57 +2001,57 @@
       <c r="P11" t="s">
         <v>74</v>
       </c>
+      <c r="Q11" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R11" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="T11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V11" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="U11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="X11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y11" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z11" s="9">
+        <v>99</v>
+      </c>
+      <c r="Y11" s="9">
         <v>2007</v>
       </c>
+      <c r="Z11" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AA11" s="9" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="AB11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC11" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD11" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE11" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF11" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG11" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2096,57 +2100,57 @@
       <c r="P12" t="s">
         <v>75</v>
       </c>
+      <c r="Q12" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="R12" s="13" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S12" s="13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="T12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="U12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V12" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="U12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="W12" s="13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="X12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z12" s="13">
+        <v>99</v>
+      </c>
+      <c r="Y12" s="13">
         <v>2007</v>
       </c>
+      <c r="Z12" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="AA12" s="13" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="AB12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD12" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE12" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF12" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG12" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2195,57 +2199,57 @@
       <c r="P13" t="s">
         <v>74</v>
       </c>
+      <c r="Q13" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R13" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="T13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="U13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V13" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="U13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="X13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z13" s="9">
+        <v>99</v>
+      </c>
+      <c r="Y13" s="9">
         <v>2007</v>
       </c>
+      <c r="Z13" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AA13" s="9" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="AB13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD13" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE13" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF13" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG13" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2294,57 +2298,57 @@
       <c r="P14" t="s">
         <v>82</v>
       </c>
+      <c r="Q14" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="R14" s="13" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S14" s="13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="T14" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="U14" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V14" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="U14" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="W14" s="13" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="X14" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y14" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z14" s="13">
+        <v>99</v>
+      </c>
+      <c r="Y14" s="13">
         <v>2007</v>
       </c>
+      <c r="Z14" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="AA14" s="13" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="AB14" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC14" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD14" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE14" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF14" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG14" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG14" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2393,57 +2397,57 @@
       <c r="P15" t="s">
         <v>83</v>
       </c>
+      <c r="Q15" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="R15" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="T15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="U15" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="V15" s="16" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="U15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="X15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y15" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z15" s="9">
+        <v>99</v>
+      </c>
+      <c r="Y15" s="9">
         <v>2007</v>
       </c>
+      <c r="Z15" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="AA15" s="9" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="AB15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC15" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD15" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AE15" s="9" t="s">
         <v>102</v>
       </c>
       <c r="AF15" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG15" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2492,57 +2496,57 @@
       <c r="P16" t="s">
         <v>84</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="Q16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="13" t="s">
+      <c r="R16" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="T16" s="10" t="s">
+      <c r="S16" s="10" t="s">
         <v>107</v>
       </c>
+      <c r="T16" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="U16" s="13" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="V16" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="W16" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="X16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y16" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z16" s="13">
+        <v>99</v>
+      </c>
+      <c r="Y16" s="13">
         <v>2012</v>
       </c>
+      <c r="Z16" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="AA16" s="13" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="AB16" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC16" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD16" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="AE16" s="13" t="s">
         <v>102</v>
       </c>
       <c r="AF16" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG16" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG16" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2591,58 +2595,58 @@
       <c r="P17" t="s">
         <v>85</v>
       </c>
-      <c r="R17" s="17" t="s">
+      <c r="Q17" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="18" t="s">
+      <c r="R17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="T17" s="17" t="s">
+      <c r="S17" s="17" t="s">
         <v>59</v>
       </c>
+      <c r="T17" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="U17" s="18" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="V17" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="W17" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="W17" s="18" t="s">
-        <v>99</v>
-      </c>
       <c r="X17" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y17" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z17" s="18">
+        <v>99</v>
+      </c>
+      <c r="Y17" s="18">
         <v>2012</v>
       </c>
+      <c r="Z17" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="AA17" s="18" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="AB17" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC17" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD17" s="18"/>
+        <v>99</v>
+      </c>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18" t="s">
+        <v>102</v>
+      </c>
       <c r="AE17" s="18" t="s">
         <v>102</v>
       </c>
       <c r="AF17" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG17" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG17" s="4" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Y1:Y5 AA1:AA5 Y7 AA7 AC1:AC1048576 Y9:Y1048576 U1:U1048576 W1:W1048576 AA9:AA1048576 S1:S1048576 AH1:AH1048576">
+  <conditionalFormatting sqref="X1:X5 Z1:Z5 X7 Z7 AB1:AB1048576 X9:X1048576 T1:T1048576 V1:V1048576 Z9:Z1048576 R1:R1048576 AG1:AG1048576 AH1">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"updated"</formula>
     </cfRule>
@@ -2650,7 +2654,7 @@
       <formula>"filled in"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y6 Y8">
+  <conditionalFormatting sqref="X6 X8">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"updated"</formula>
     </cfRule>
@@ -2658,7 +2662,7 @@
       <formula>"filled in"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA6 AA8">
+  <conditionalFormatting sqref="Z6 Z8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"updated"</formula>
     </cfRule>

</xml_diff>